<commit_message>
new 100+ data responses
</commit_message>
<xml_diff>
--- a/datasets/rawdata.xlsx
+++ b/datasets/rawdata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="277">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="470">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -866,6 +866,585 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Card;Strategy;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">art P-12</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Luck;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">slap jack, rat slap, kings in the corner</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Animals;Auction;Card;Exploration;Fantasy;Farming;Horror;Luck;Medieval;Racing;Roll and Move ;Role-Playing ;Trains;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Chemistry either organic or inorganic</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Puzzle-Solving;Luck;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Battleships, Apples to Apples, Cards Against Humanity</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Exploration;Fantasy;Horror;Puzzle;Science Fiction;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">24</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Math</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Deck-Building ;Card;Deduction;Party ;Social Deduction/Hidden Role;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Luck;Strategy;Heavy/Immersive Theming;Party/Low-Stakes;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Hues and cues, stoned drunk or stupid, cards against humanity, DnD</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Card;Fighting;Luck;Medieval;Party ;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Electrical Engineering</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Luck;Conflict/Competition;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">“Munchkin”, “Jenga”</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Tile-Laying ;Territory Building;Strategy;Fantasy;Cooperative ;Card;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Seeking employment</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Undecided but leaning towards engineering</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Strategy;Social Deduction/Hidden Role;Puzzle-Solving;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Monopoly, poker, exploding kittens, war, hearts, cards against humanity, chess</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Cooperative ;Deck-Building ;Economic;Farming;Luck;Party ;Strategy;Territory Building;War ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Medicine </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Luck;Strategy;Puzzle-Solving;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Card;Cooperative ;Fantasy;Fighting;Horror;Luck;Medieval;Political;Puzzle;Racing;Role-Playing ;Science Fiction;Strategy;War ;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">rec management </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Economics </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Luck;Strategy;Trivia;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Texas holdem </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Sports;World War II;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">29</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Geology</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Strategy;Luck;Trivia;Puzzle-Solving;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Catan, exploding kittens, wingspan, cribbage</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Animals;Card Drafting;Card;Civilization;Deck-Building ;Cooperative ;Deduction;Educational;Exploration;Fantasy;Farming;Fighting;Medieval;Memory;Luck;Miniatures;Party ;Pirates;Political;Puzzle;Roll and Move ;Role-Playing ;Science Fiction;Strategy;Trains;Tile-Laying ;Transportation;Travel;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">25</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Strategy;Puzzle-Solving;Trivia;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Miniatures;Auction;Card;Cooperative ;Economic;Fantasy;Puzzle;Tile-Laying ;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">28</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Strategy;Puzzle-Solving;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Uno, pandemic, catan, mancala, ticket to ride, </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Cooperative ;Civilization;Deck-Building ;Puzzle;Racing;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">26</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Strategy;Puzzle-Solving;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Wingspan, Chess, Catan, Ragnarok, Go, Unstable Unicorns, Uno, Brew, Dicecapades</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Animals;Fantasy;Fighting;Role-Playing ;Roll and Move ;Puzzle;Tile-Laying ;Strategy;Trivia;Travel;War ;Word ;Trains;Territory Building;Social Deduction/Hidden Role;Pirates;Exploration;Educational;Deduction;Civilization;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">White;Black or African American;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Cooperation;Social Deduction/Hidden Role;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">“Uno”,”monopoly”</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Card;Fantasy;Luck;Party ;War ;World War II;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Visual Journalism </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Strategy;Puzzle-Solving;Trivia;Party/Low-Stakes;Social Deduction/Hidden Role;Heavy/Immersive Theming;Luck;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">UNO, Red Dragon Inn, Sorry, The Thing, Betrayal at the House on the Hill, Forbidden Series, Clue, Root, Risk, Axis &amp; Allies, Machi Koro, Pit, Apples to Apples, Battle Ball</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Exploration;Fantasy;Fighting;Luck;Memory;Party ;Miniatures;Puzzle;Racing;Sports;Science Fiction;Strategy;Territory Building;Trains;Transportation;Travel;Trivia;War ;World War II;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Puzzle-Solving;Strategy;Luck;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Uno, Oofta, Kings in the corners, aggravation, clue, unstable unicorns, settlers of Catan, exploding kittens</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Animals;Card;Civilization;Cooperative ;Deduction;Fantasy;Exploration;Medieval;Miniatures;Pirates;Puzzle;Racing;Roll and Move ;Role-Playing ;Territory Building;Travel;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Seasonal worker during the summer</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Environmental studies </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Strategy;Social Deduction/Hidden Role;Heavy/Immersive Theming;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Game 1 monopoly  game 2 mancola game 3 uno game 4 secret hitler</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Civilization;Card;Deck-Building ;Fantasy;Fighting;Farming;Medieval;Miniatures;Role-Playing ;Science Fiction;Strategy;Territory Building;War ;World War II;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Biology/Math</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Strategy;Social Deduction/Hidden Role;Puzzle-Solving;Party/Low-Stakes;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Secret Hitler, codenames, uno, 3-13, Betrayal at the House on the Hill</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Deck-Building ;Deduction;Horror;Memory;Party ;Puzzle;Roll and Move ;Racing;Strategy;Tile-Laying ;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Puzzle-Solving;Trivia;Party/Low-Stakes;Strategy;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Taboo, scrabble, chess</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperative ;Strategy;Trivia;Word ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">WWU Faculty Member</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Yugioh </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Behavioral Neuroscience</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Puzzle-Solving;Trivia;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Code Names</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Card;Cooperative ;Deduction;Memory;Party ;Puzzle;Roll and Move ;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Hispanic or Latino;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Employed full-time</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Electrical Engineering </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Strategy;Puzzle-Solving;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Catan, Trivial Pursuit, Sequence, Phase 10, Ticket to Ride</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Card;Fighting;Horror;Medieval;Memory;Party ;Puzzle;Racing;Science Fiction;Sports;Trivia;War ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Buddhism</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Computer Science</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Animals;Auction;Card;Card Drafting;Civilization;Cooperative ;Deck-Building ;Deduction;Economic;Educational;Exploration;Fantasy;Farming;Fighting;Horror;Luck;Medieval;Memory;Miniatures;Party ;Pirates;Political;Puzzle;Racing;Roll and Move ;Science Fiction;Role-Playing ;Strategy;Territory Building;Sports;Social Deduction/Hidden Role;Tile-Laying ;Trains;Transportation;Travel;War ;World War II;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Geology (paleoclimate)</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Trivia;Conflict/Competition;Puzzle-Solving;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Uno, Battleship, Castle Tower, Mahjong, Chess,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Trivia;Social Deduction/Hidden Role;Cooperative ;Horror;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Electrical engineering</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Luck;Strategy;Social Deduction/Hidden Role;Heavy/Immersive Theming;Puzzle-Solving;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Card Drafting;Card;Civilization;Cooperative ;Deck-Building ;Deduction;Economic;Exploration;Fantasy;Fighting;Farming;Horror;Medieval;Miniatures;Party ;Pirates;Political;Puzzle;Racing;Roll and Move ;Role-Playing ;Science Fiction;Social Deduction/Hidden Role;Strategy;Territory Building;Tile-Laying ;Trains;Transportation;Travel;War ;Worker Placement;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Marine Biology and Theater Production</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Party/Low-Stakes;Trivia;Puzzle-Solving;Heavy/Immersive Theming;Social Deduction/Hidden Role;Strategy;Luck;Conflict/Competition;Cooperation;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Card Drafting;Card;Cooperative ;Deduction;Exploration;Fighting;Horror;Luck;Memory;Party ;Pirates;Puzzle;Racing;Roll and Move ;Role-Playing ;Science Fiction;Social Deduction/Hidden Role;Sports;Strategy;Territory Building;Transportation;Travel;Word ;World War II;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Computer science</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Strategy;Cooperation;Heavy/Immersive Theming;Conflict/Competition;Luck;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">“Dungeons &amp; Dragons”</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Fighting;Medieval;Pirates;Role-Playing ;Science Fiction;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Strategy;Puzzle-Solving;Cooperation;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Spite and Malice, Azul, Quirkle, clue, settlers of catan</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Card;Cooperative ;Deduction;Horror;Luck;Memory;Racing;Puzzle;Roll and Move ;Science Fiction;Territory Building;Strategy;Tile-Laying ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Anthropology</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Strategy;Luck;Social Deduction/Hidden Role;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Clue, card wars, uno, Catan, chess</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Card;Civilization;Deduction;Political;Territory Building;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Biology </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Management information systems </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Strategy;Luck;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Variations Settlers of Catan, magic the gathering, chess, </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Card;Civilization;Deck-Building ;Fantasy;Fighting;Party ;Sports;War ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">marine bio</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Strategy;Luck;Conflict/Competition;Social Deduction/Hidden Role;Trivia;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">monopoly, life, clue, go fish, aggravation</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Animals;Memory;Party ;Pirates;Racing;Roll and Move ;Social Deduction/Hidden Role;Strategy;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Environmental Studies</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Luck;Strategy;Conflict/Competition;Party/Low-Stakes;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Monopoly, poker, go fish, kanasta</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Card Drafting;Card;Civilization;Deck-Building ;Luck;Party ;Political;Trivia;War ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">History/Holocaust &amp; Genocide Studies</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Strategy;Social Deduction/Hidden Role;Heavy/Immersive Theming;Puzzle-Solving;Trivia;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Game 1: Dead of Winter Game 2: Drunk Stoned or Stupid Game 3: Pandemic Game 4: Uno</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Cooperative ;Deduction;Educational;Exploration;Fantasy;Farming;Fighting;Horror;Medieval;Party ;Pirates;Puzzle;Roll and Move ;Role-Playing ;Science Fiction;Social Deduction/Hidden Role;Strategy;Tile-Laying ;Travel;Trivia;Worker Placement;Word ;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SPED &amp; ELED</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Luck;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Game one: uno, game two: cribbage, game three: trouble, game four: sorry, game five: parcheesi, game six: monopoly, game seven: scrabble</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Social Deduction/Hidden Role;Party/Low-Stakes;Puzzle-Solving;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">“Monopoly”, “Cards Against Humanity”, “Jackbox”</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Social Deduction/Hidden Role;Trivia;Political;Party ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Gender-fluid </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Trivia;Party/Low-Stakes;Puzzle-Solving;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Party ;Puzzle;Strategy;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Genderfluid</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Visual Journalism</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Strategy;Puzzle-Solving;Trivia;Party/Low-Stakes;Luck;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">"Speed (card game)", "Ticket to Ride", "Telestrations", "Smallworld", "Exploding Kittens"</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Fantasy;Memory;Party ;Puzzle;Word ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Elementary education</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Party/Low-Stakes;Trivia;Luck;Strategy;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">The state game, mancala, bullsh*t (the card game), life</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Roll and Move ;Party ;Educational;Strategy;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">White;Native Hawaiian or Pacific Islander;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Anthropology, Communication Studies</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Uno</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Gender queer</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Asian;Filipino;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Theatre</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Social Deduction/Hidden Role;Heavy/Immersive Theming;Puzzle-Solving;Trivia;Strategy;Party/Low-Stakes;Luck;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">MTG, Secret Hitler (Mafia), DnD, exploding kittens, You have grabs, monopoly</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Card Drafting;Card;Deck-Building ;Deduction;Educational;Fantasy;Exploration;Fighting;Farming;Horror;Luck;Party ;Pirates;Political;Role-Playing ;Science Fiction;Social Deduction/Hidden Role;Strategy;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Studio Art</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Uno, Dune, monopoly, sorry, exploding kittens, sushi go</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Cooperative ;Exploration;Horror;Puzzle;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Urban Planning and Sustainable Development</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Cooperation;Luck;Strategy;Heavy/Immersive Theming;Puzzle-Solving;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Uno, poker, mancala, scattegories, cards against humanity, chess</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Animals;Auction;Civilization;Cooperative ;Card;Fantasy;Farming;Fighting;Luck;Political;Pirates;Party ;Roll and Move ;Science Fiction;Sports;Trains;Transportation;Travel;War ;Zombies;Word ;Strategy;Puzzle;Racing;Medieval;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Urban Planning and Sustainable Development </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Trivia;Puzzle-Solving;Luck;Strategy;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">“ Cribbage”, “uno”, “Cards Agains Humanity”, “Checkers”, “Spoons”</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Luck;Puzzle;Roll and Move ;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Luck;Social Deduction/Hidden Role;Strategy;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Binding of Isaac card game </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Horror;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Strategy;Social Deduction/Hidden Role;Trivia;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Game 1: settlers of Catan Game 2: uno Game 3:BS (card game) </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Animals;Auction;Card Drafting;Card;Civilization;Cooperative ;Deck-Building ;Exploration;Fantasy;Farming;Fighting;Horror;Luck;Medieval;Memory;Miniatures;Party ;Pirates;Political;Puzzle;Racing;Roll and Move ;Role-Playing ;Science Fiction;Social Deduction/Hidden Role;Sports;Strategy;Territory Building;Tile-Laying ;Trains;Transportation;Travel;Trivia;War ;Worker Placement;Word ;World War II;Zombies;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Science</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">History </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Strategy;Cooperation;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Battleship</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Economic;Fighting;Science Fiction;War ;World War II;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Art and design </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cooperation;Conflict/Competition;Luck;Strategy;Puzzle-Solving;Trivia;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Black or African American;White;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Kinesiology </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Strategy;Luck;Heavy/Immersive Theming;Puzzle-Solving;Trivia;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">clue, tunk, poker, chess,</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Abstract Strategy;Adventure;Animals;Card;Cooperative ;Fantasy;Fighting;Horror;Luck;Memory;Party ;Puzzle;Sports;Strategy;Travel;Trivia;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Environmental Science </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Strategy;Luck;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Magic The Gathering, Catan</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Adventure;Card;Card Drafting;Civilization;Cooperative ;Deck-Building ;Fantasy;Exploration;Fighting;Medieval;Memory;Party ;Roll and Move ;Racing;Role-Playing ;Science Fiction;Strategy;Tile-Laying ;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Spanish </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Party/Low-Stakes;Conflict/Competition;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">monopoly, ticket to ride, jenga, scrabble, </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Card;Exploration;Memory;Party ;Puzzle;Sports;Trains;Travel;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Biochemistry </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Conflict/Competition;Cooperation;Party/Low-Stakes;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Catan</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Animals;Adventure;Card Drafting;Card;Civilization;Cooperative ;</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -962,8 +1541,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:V57" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:V57"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:V109" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:V109"/>
   <x:tableColumns count="22">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
@@ -4919,11 +5498,3301 @@
         <x:v>276</x:v>
       </x:c>
     </x:row>
+    <x:row r="58" hidden="0">
+      <x:c r="A58">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B58" s="2">
+        <x:v>45243.8322916667</x:v>
+      </x:c>
+      <x:c r="C58" s="2">
+        <x:v>45243.8344791667</x:v>
+      </x:c>
+      <x:c r="D58" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E58" s="10" t="s"/>
+      <x:c r="F58" s="2"/>
+      <x:c r="G58" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H58" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I58" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J58" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K58" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L58" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M58" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N58" s="10" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="O58" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P58" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q58" s="10" t="s">
+        <x:v>189</x:v>
+      </x:c>
+      <x:c r="R58" s="10" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="S58" s="10" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="T58" s="10" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="U58">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V58" s="10" t="s">
+        <x:v>280</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" hidden="0">
+      <x:c r="A59">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B59" s="2">
+        <x:v>45243.8970486111</x:v>
+      </x:c>
+      <x:c r="C59" s="2">
+        <x:v>45243.8996296296</x:v>
+      </x:c>
+      <x:c r="D59" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E59" s="10" t="s"/>
+      <x:c r="F59" s="2"/>
+      <x:c r="G59" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H59" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I59" s="7" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="J59" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K59" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L59" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M59" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N59" s="10" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="O59" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P59" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q59" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R59" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S59" s="10" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="T59" s="10" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="U59">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V59" s="10" t="s">
+        <x:v>284</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" hidden="0">
+      <x:c r="A60">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B60" s="2">
+        <x:v>45244.4829282407</x:v>
+      </x:c>
+      <x:c r="C60" s="2">
+        <x:v>45244.4855208333</x:v>
+      </x:c>
+      <x:c r="D60" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E60" s="10" t="s"/>
+      <x:c r="F60" s="2"/>
+      <x:c r="G60" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H60" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I60" s="7" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="J60" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K60" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L60" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M60" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N60" s="10" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="O60" s="10" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="P60" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="Q60" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R60" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S60" s="10" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="T60" s="10" t="s"/>
+      <x:c r="U60">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="V60" s="10" t="s">
+        <x:v>287</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" hidden="0">
+      <x:c r="A61">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B61" s="2">
+        <x:v>45245.5809375</x:v>
+      </x:c>
+      <x:c r="C61" s="2">
+        <x:v>45245.5825231481</x:v>
+      </x:c>
+      <x:c r="D61" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E61" s="10" t="s"/>
+      <x:c r="F61" s="2"/>
+      <x:c r="G61" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H61" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I61" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J61" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K61" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L61" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M61" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="N61" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="O61" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P61" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q61" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R61" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S61" s="10" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="T61" s="10" t="s">
+        <x:v>289</x:v>
+      </x:c>
+      <x:c r="U61">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V61" s="10" t="s">
+        <x:v>290</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" hidden="0">
+      <x:c r="A62">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B62" s="2">
+        <x:v>45245.6174074074</x:v>
+      </x:c>
+      <x:c r="C62" s="2">
+        <x:v>45245.6223726852</x:v>
+      </x:c>
+      <x:c r="D62" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E62" s="10" t="s"/>
+      <x:c r="F62" s="2"/>
+      <x:c r="G62" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H62" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I62" s="10" t="s"/>
+      <x:c r="J62" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K62" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L62" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M62" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N62" s="10" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="O62" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="P62" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q62" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R62" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S62" s="10" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="T62" s="10" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="U62">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="V62" s="10" t="s">
+        <x:v>294</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" hidden="0">
+      <x:c r="A63">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B63" s="2">
+        <x:v>45246.489212963</x:v>
+      </x:c>
+      <x:c r="C63" s="2">
+        <x:v>45246.4925115741</x:v>
+      </x:c>
+      <x:c r="D63" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E63" s="10" t="s"/>
+      <x:c r="F63" s="2"/>
+      <x:c r="G63" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H63" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I63" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J63" s="10" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="K63" s="10" t="s">
+        <x:v>295</x:v>
+      </x:c>
+      <x:c r="L63" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M63" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N63" s="10" t="s">
+        <x:v>296</x:v>
+      </x:c>
+      <x:c r="O63" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P63" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q63" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R63" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S63" s="10" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="T63" s="10" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="U63">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="V63" s="10" t="s">
+        <x:v>299</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" hidden="0">
+      <x:c r="A64">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B64" s="2">
+        <x:v>45246.5026388889</x:v>
+      </x:c>
+      <x:c r="C64" s="2">
+        <x:v>45246.5049421296</x:v>
+      </x:c>
+      <x:c r="D64" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E64" s="10" t="s"/>
+      <x:c r="F64" s="2"/>
+      <x:c r="G64" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H64" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I64" s="7" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="J64" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K64" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L64" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M64" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N64" s="10" t="s">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="O64" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P64" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="Q64" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R64" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S64" s="10" t="s">
+        <x:v>301</x:v>
+      </x:c>
+      <x:c r="T64" s="10" t="s"/>
+      <x:c r="U64">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V64" s="10" t="s">
+        <x:v>302</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" hidden="0">
+      <x:c r="A65">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B65" s="2">
+        <x:v>45246.5054398148</x:v>
+      </x:c>
+      <x:c r="C65" s="2">
+        <x:v>45246.5067476852</x:v>
+      </x:c>
+      <x:c r="D65" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E65" s="10" t="s"/>
+      <x:c r="F65" s="2"/>
+      <x:c r="G65" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H65" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I65" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J65" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K65" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L65" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M65" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N65" s="10" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="O65" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="P65" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="Q65" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R65" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S65" s="10" t="s">
+        <x:v>249</x:v>
+      </x:c>
+      <x:c r="T65" s="10" t="s"/>
+      <x:c r="U65">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V65" s="10" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" hidden="0">
+      <x:c r="A66">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B66" s="2">
+        <x:v>45246.5050115741</x:v>
+      </x:c>
+      <x:c r="C66" s="2">
+        <x:v>45246.5069907407</x:v>
+      </x:c>
+      <x:c r="D66" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E66" s="10" t="s"/>
+      <x:c r="F66" s="2"/>
+      <x:c r="G66" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H66" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I66" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J66" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K66" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L66" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="M66" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="N66" s="10" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="O66" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P66" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q66" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R66" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S66" s="10" t="s">
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="T66" s="10" t="s">
+        <x:v>306</x:v>
+      </x:c>
+      <x:c r="U66">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="V66" s="10" t="s">
+        <x:v>307</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" hidden="0">
+      <x:c r="A67">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B67" s="2">
+        <x:v>45246.5041087963</x:v>
+      </x:c>
+      <x:c r="C67" s="2">
+        <x:v>45246.5077314815</x:v>
+      </x:c>
+      <x:c r="D67" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E67" s="10" t="s"/>
+      <x:c r="F67" s="2"/>
+      <x:c r="G67" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H67" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I67" s="7" t="s">
+        <x:v>308</x:v>
+      </x:c>
+      <x:c r="J67" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K67" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L67" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M67" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N67" s="10" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="O67" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P67" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q67" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R67" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S67" s="10" t="s">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="T67" s="10" t="s">
+        <x:v>311</x:v>
+      </x:c>
+      <x:c r="U67">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="V67" s="10" t="s">
+        <x:v>312</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" hidden="0">
+      <x:c r="A68">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B68" s="2">
+        <x:v>45246.5061111111</x:v>
+      </x:c>
+      <x:c r="C68" s="2">
+        <x:v>45246.5078125</x:v>
+      </x:c>
+      <x:c r="D68" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E68" s="10" t="s"/>
+      <x:c r="F68" s="2"/>
+      <x:c r="G68" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H68" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I68" s="7" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J68" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K68" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L68" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M68" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N68" s="10" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="O68" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P68" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q68" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R68" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S68" s="10" t="s">
+        <x:v>314</x:v>
+      </x:c>
+      <x:c r="T68" s="10" t="s"/>
+      <x:c r="U68">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V68" s="10" t="s">
+        <x:v>315</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="69" hidden="0">
+      <x:c r="A69">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B69" s="2">
+        <x:v>45246.5039351852</x:v>
+      </x:c>
+      <x:c r="C69" s="2">
+        <x:v>45246.5085532407</x:v>
+      </x:c>
+      <x:c r="D69" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E69" s="10" t="s"/>
+      <x:c r="F69" s="2"/>
+      <x:c r="G69" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H69" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I69" s="7" t="s">
+        <x:v>316</x:v>
+      </x:c>
+      <x:c r="J69" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K69" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L69" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M69" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N69" s="10" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="O69" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P69" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q69" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R69" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S69" s="10" t="s">
+        <x:v>317</x:v>
+      </x:c>
+      <x:c r="T69" s="10" t="s">
+        <x:v>318</x:v>
+      </x:c>
+      <x:c r="U69">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="V69" s="10" t="s">
+        <x:v>319</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" hidden="0">
+      <x:c r="A70">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B70" s="2">
+        <x:v>45246.5040277778</x:v>
+      </x:c>
+      <x:c r="C70" s="2">
+        <x:v>45246.5088194444</x:v>
+      </x:c>
+      <x:c r="D70" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E70" s="10" t="s"/>
+      <x:c r="F70" s="2"/>
+      <x:c r="G70" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H70" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="I70" s="7" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="J70" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K70" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L70" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M70" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N70" s="10" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="O70" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P70" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q70" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R70" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S70" s="10" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="T70" s="10" t="s">
+        <x:v>322</x:v>
+      </x:c>
+      <x:c r="U70">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="V70" s="10" t="s">
+        <x:v>323</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" hidden="0">
+      <x:c r="A71">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B71" s="2">
+        <x:v>45246.5058217593</x:v>
+      </x:c>
+      <x:c r="C71" s="2">
+        <x:v>45246.509212963</x:v>
+      </x:c>
+      <x:c r="D71" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E71" s="10" t="s"/>
+      <x:c r="F71" s="2"/>
+      <x:c r="G71" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H71" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I71" s="7" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="J71" s="10" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="K71" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L71" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M71" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N71" s="10" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="O71" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P71" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q71" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R71" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S71" s="10" t="s">
+        <x:v>325</x:v>
+      </x:c>
+      <x:c r="T71" s="10" t="s">
+        <x:v>326</x:v>
+      </x:c>
+      <x:c r="U71">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="V71" s="10" t="s">
+        <x:v>327</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" hidden="0">
+      <x:c r="A72">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B72" s="2">
+        <x:v>45246.5077199074</x:v>
+      </x:c>
+      <x:c r="C72" s="2">
+        <x:v>45246.5118518519</x:v>
+      </x:c>
+      <x:c r="D72" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E72" s="10" t="s"/>
+      <x:c r="F72" s="2"/>
+      <x:c r="G72" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H72" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I72" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J72" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K72" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L72" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M72" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N72" s="10" t="s">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="O72" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P72" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="Q72" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R72" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S72" s="10" t="s">
+        <x:v>329</x:v>
+      </x:c>
+      <x:c r="T72" s="10" t="s">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="U72">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="V72" s="10" t="s">
+        <x:v>331</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" hidden="0">
+      <x:c r="A73">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B73" s="2">
+        <x:v>45246.5054166667</x:v>
+      </x:c>
+      <x:c r="C73" s="2">
+        <x:v>45246.512037037</x:v>
+      </x:c>
+      <x:c r="D73" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E73" s="10" t="s"/>
+      <x:c r="F73" s="2"/>
+      <x:c r="G73" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H73" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I73" s="7" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="J73" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K73" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L73" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M73" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N73" s="10" t="s"/>
+      <x:c r="O73" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P73" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q73" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R73" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S73" s="10" t="s">
+        <x:v>332</x:v>
+      </x:c>
+      <x:c r="T73" s="10" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="U73">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="V73" s="10" t="s">
+        <x:v>334</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" hidden="0">
+      <x:c r="A74">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="B74" s="2">
+        <x:v>45246.5030208333</x:v>
+      </x:c>
+      <x:c r="C74" s="2">
+        <x:v>45246.5138310185</x:v>
+      </x:c>
+      <x:c r="D74" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E74" s="10" t="s"/>
+      <x:c r="F74" s="2"/>
+      <x:c r="G74" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H74" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I74" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J74" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K74" s="10" t="s">
+        <x:v>335</x:v>
+      </x:c>
+      <x:c r="L74" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M74" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N74" s="10" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="O74" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P74" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q74" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R74" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S74" s="10" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="T74" s="10" t="s">
+        <x:v>338</x:v>
+      </x:c>
+      <x:c r="U74">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="V74" s="10" t="s">
+        <x:v>339</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" hidden="0">
+      <x:c r="A75">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B75" s="2">
+        <x:v>45246.5227662037</x:v>
+      </x:c>
+      <x:c r="C75" s="2">
+        <x:v>45246.5257523148</x:v>
+      </x:c>
+      <x:c r="D75" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E75" s="10" t="s"/>
+      <x:c r="F75" s="2"/>
+      <x:c r="G75" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H75" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I75" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J75" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K75" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L75" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M75" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N75" s="10" t="s">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="O75" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P75" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q75" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R75" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S75" s="10" t="s">
+        <x:v>341</x:v>
+      </x:c>
+      <x:c r="T75" s="10" t="s">
+        <x:v>342</x:v>
+      </x:c>
+      <x:c r="U75">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V75" s="10" t="s">
+        <x:v>343</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" hidden="0">
+      <x:c r="A76">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="B76" s="2">
+        <x:v>45246.5233101852</x:v>
+      </x:c>
+      <x:c r="C76" s="2">
+        <x:v>45246.5258449074</x:v>
+      </x:c>
+      <x:c r="D76" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E76" s="10" t="s"/>
+      <x:c r="F76" s="2"/>
+      <x:c r="G76" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H76" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I76" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J76" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K76" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L76" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M76" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N76" s="10" t="s"/>
+      <x:c r="O76" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P76" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q76" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R76" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S76" s="10" t="s">
+        <x:v>344</x:v>
+      </x:c>
+      <x:c r="T76" s="10" t="s">
+        <x:v>345</x:v>
+      </x:c>
+      <x:c r="U76">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="V76" s="10" t="s">
+        <x:v>346</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="77" hidden="0">
+      <x:c r="A77">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="B77" s="2">
+        <x:v>45246.5254513889</x:v>
+      </x:c>
+      <x:c r="C77" s="2">
+        <x:v>45246.5268055556</x:v>
+      </x:c>
+      <x:c r="D77" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E77" s="10" t="s"/>
+      <x:c r="F77" s="2"/>
+      <x:c r="G77" s="10" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="H77" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I77" s="7" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="J77" s="10" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="K77" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L77" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M77" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N77" s="10" t="s">
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="O77" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="P77" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="Q77" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R77" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="S77" s="10" t="s">
+        <x:v>348</x:v>
+      </x:c>
+      <x:c r="T77" s="10" t="s">
+        <x:v>349</x:v>
+      </x:c>
+      <x:c r="U77">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V77" s="10" t="s"/>
+    </x:row>
+    <x:row r="78" hidden="0">
+      <x:c r="A78">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="B78" s="2">
+        <x:v>45246.5260416667</x:v>
+      </x:c>
+      <x:c r="C78" s="2">
+        <x:v>45246.5276736111</x:v>
+      </x:c>
+      <x:c r="D78" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E78" s="10" t="s"/>
+      <x:c r="F78" s="2"/>
+      <x:c r="G78" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H78" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I78" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J78" s="10" t="s">
+        <x:v>324</x:v>
+      </x:c>
+      <x:c r="K78" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L78" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M78" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N78" s="10" t="s">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="O78" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P78" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q78" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R78" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="S78" s="10" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="T78" s="10" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="U78">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="V78" s="10" t="s">
+        <x:v>353</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" hidden="0">
+      <x:c r="A79">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="B79" s="2">
+        <x:v>45246.5267361111</x:v>
+      </x:c>
+      <x:c r="C79" s="2">
+        <x:v>45246.5295833333</x:v>
+      </x:c>
+      <x:c r="D79" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E79" s="10" t="s"/>
+      <x:c r="F79" s="2"/>
+      <x:c r="G79" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H79" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I79" s="7" t="s">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="J79" s="10" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="K79" s="10" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="L79" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M79" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N79" s="10" t="s">
+        <x:v>356</x:v>
+      </x:c>
+      <x:c r="O79" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P79" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q79" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="R79" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S79" s="10" t="s">
+        <x:v>357</x:v>
+      </x:c>
+      <x:c r="T79" s="10" t="s">
+        <x:v>358</x:v>
+      </x:c>
+      <x:c r="U79">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V79" s="10" t="s">
+        <x:v>359</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" hidden="0">
+      <x:c r="A80">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="B80" s="2">
+        <x:v>45246.5286689815</x:v>
+      </x:c>
+      <x:c r="C80" s="2">
+        <x:v>45246.5298032407</x:v>
+      </x:c>
+      <x:c r="D80" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E80" s="10" t="s"/>
+      <x:c r="F80" s="2"/>
+      <x:c r="G80" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H80" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I80" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J80" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K80" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L80" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M80" s="10" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="N80" s="10" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="O80" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P80" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q80" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R80" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S80" s="10" t="s">
+        <x:v>237</x:v>
+      </x:c>
+      <x:c r="T80" s="10" t="s"/>
+      <x:c r="U80">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V80" s="10" t="s">
+        <x:v>362</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" hidden="0">
+      <x:c r="A81">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="B81" s="2">
+        <x:v>45246.5260416667</x:v>
+      </x:c>
+      <x:c r="C81" s="2">
+        <x:v>45246.5312152778</x:v>
+      </x:c>
+      <x:c r="D81" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E81" s="10" t="s"/>
+      <x:c r="F81" s="2"/>
+      <x:c r="G81" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H81" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I81" s="7" t="s">
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J81" s="10" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="K81" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L81" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M81" s="10" t="s">
+        <x:v>214</x:v>
+      </x:c>
+      <x:c r="N81" s="10" t="s">
+        <x:v>363</x:v>
+      </x:c>
+      <x:c r="O81" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P81" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q81" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R81" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S81" s="10" t="s">
+        <x:v>364</x:v>
+      </x:c>
+      <x:c r="T81" s="10" t="s">
+        <x:v>365</x:v>
+      </x:c>
+      <x:c r="U81">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="V81" s="10" t="s">
+        <x:v>366</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" hidden="0">
+      <x:c r="A82">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="B82" s="2">
+        <x:v>45246.5333217593</x:v>
+      </x:c>
+      <x:c r="C82" s="2">
+        <x:v>45246.5349884259</x:v>
+      </x:c>
+      <x:c r="D82" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E82" s="10" t="s"/>
+      <x:c r="F82" s="2"/>
+      <x:c r="G82" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H82" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="I82" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J82" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K82" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L82" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M82" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N82" s="10" t="s">
+        <x:v>367</x:v>
+      </x:c>
+      <x:c r="O82" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P82" s="10" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="Q82" s="10" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="R82" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S82" s="10" t="s">
+        <x:v>368</x:v>
+      </x:c>
+      <x:c r="T82" s="10" t="s"/>
+      <x:c r="U82">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="V82" s="10" t="s">
+        <x:v>369</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" hidden="0">
+      <x:c r="A83">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="B83" s="2">
+        <x:v>45246.5334953704</x:v>
+      </x:c>
+      <x:c r="C83" s="2">
+        <x:v>45246.5360648148</x:v>
+      </x:c>
+      <x:c r="D83" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E83" s="10" t="s"/>
+      <x:c r="F83" s="2"/>
+      <x:c r="G83" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H83" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I83" s="7" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="J83" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K83" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L83" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M83" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N83" s="10" t="s">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="O83" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P83" s="10" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="Q83" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R83" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S83" s="10" t="s">
+        <x:v>371</x:v>
+      </x:c>
+      <x:c r="T83" s="10" t="s"/>
+      <x:c r="U83">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="V83" s="10" t="s">
+        <x:v>372</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" hidden="0">
+      <x:c r="A84">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="B84" s="2">
+        <x:v>45246.5350694444</x:v>
+      </x:c>
+      <x:c r="C84" s="2">
+        <x:v>45246.5383680556</x:v>
+      </x:c>
+      <x:c r="D84" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E84" s="10" t="s"/>
+      <x:c r="F84" s="2"/>
+      <x:c r="G84" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H84" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I84" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J84" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K84" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L84" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M84" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N84" s="10" t="s">
+        <x:v>373</x:v>
+      </x:c>
+      <x:c r="O84" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P84" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q84" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="R84" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S84" s="10" t="s">
+        <x:v>374</x:v>
+      </x:c>
+      <x:c r="T84" s="10" t="s">
+        <x:v>375</x:v>
+      </x:c>
+      <x:c r="U84">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V84" s="10" t="s">
+        <x:v>376</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" hidden="0">
+      <x:c r="A85">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="B85" s="2">
+        <x:v>45246.5393518518</x:v>
+      </x:c>
+      <x:c r="C85" s="2">
+        <x:v>45246.5433449074</x:v>
+      </x:c>
+      <x:c r="D85" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E85" s="10" t="s"/>
+      <x:c r="F85" s="2"/>
+      <x:c r="G85" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H85" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="I85" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J85" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K85" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L85" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M85" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N85" s="10" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="O85" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P85" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q85" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R85" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S85" s="10" t="s">
+        <x:v>377</x:v>
+      </x:c>
+      <x:c r="T85" s="10" t="s">
+        <x:v>378</x:v>
+      </x:c>
+      <x:c r="U85">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="V85" s="10" t="s">
+        <x:v>379</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" hidden="0">
+      <x:c r="A86">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="B86" s="2">
+        <x:v>45246.5430555556</x:v>
+      </x:c>
+      <x:c r="C86" s="2">
+        <x:v>45246.5458333333</x:v>
+      </x:c>
+      <x:c r="D86" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E86" s="10" t="s"/>
+      <x:c r="F86" s="2"/>
+      <x:c r="G86" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H86" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I86" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J86" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K86" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L86" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M86" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N86" s="10" t="s">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="O86" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P86" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q86" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R86" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S86" s="10" t="s">
+        <x:v>381</x:v>
+      </x:c>
+      <x:c r="T86" s="10" t="s">
+        <x:v>382</x:v>
+      </x:c>
+      <x:c r="U86">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V86" s="10" t="s">
+        <x:v>383</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" hidden="0">
+      <x:c r="A87">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="B87" s="2">
+        <x:v>45246.5461574074</x:v>
+      </x:c>
+      <x:c r="C87" s="2">
+        <x:v>45246.5472800926</x:v>
+      </x:c>
+      <x:c r="D87" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E87" s="10" t="s"/>
+      <x:c r="F87" s="2"/>
+      <x:c r="G87" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H87" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I87" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J87" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K87" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L87" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M87" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N87" s="10" t="s">
+        <x:v>384</x:v>
+      </x:c>
+      <x:c r="O87" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P87" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q87" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R87" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S87" s="10" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="T87" s="10" t="s"/>
+      <x:c r="U87">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V87" s="10" t="s"/>
+    </x:row>
+    <x:row r="88" hidden="0">
+      <x:c r="A88">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="B88" s="2">
+        <x:v>45246.5465162037</x:v>
+      </x:c>
+      <x:c r="C88" s="2">
+        <x:v>45246.548587963</x:v>
+      </x:c>
+      <x:c r="D88" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E88" s="10" t="s"/>
+      <x:c r="F88" s="2"/>
+      <x:c r="G88" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H88" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I88" s="7" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J88" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K88" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L88" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M88" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N88" s="10" t="s">
+        <x:v>385</x:v>
+      </x:c>
+      <x:c r="O88" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P88" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q88" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="R88" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S88" s="10" t="s">
+        <x:v>386</x:v>
+      </x:c>
+      <x:c r="T88" s="10" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="U88">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V88" s="10" t="s">
+        <x:v>388</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" hidden="0">
+      <x:c r="A89">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="B89" s="2">
+        <x:v>45246.5612615741</x:v>
+      </x:c>
+      <x:c r="C89" s="2">
+        <x:v>45246.5628356481</x:v>
+      </x:c>
+      <x:c r="D89" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E89" s="10" t="s"/>
+      <x:c r="F89" s="2"/>
+      <x:c r="G89" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H89" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I89" s="7" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="J89" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K89" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L89" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M89" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N89" s="10" t="s">
+        <x:v>389</x:v>
+      </x:c>
+      <x:c r="O89" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P89" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q89" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R89" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S89" s="10" t="s">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="T89" s="10" t="s">
+        <x:v>391</x:v>
+      </x:c>
+      <x:c r="U89">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V89" s="10" t="s">
+        <x:v>392</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" hidden="0">
+      <x:c r="A90">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="B90" s="2">
+        <x:v>45246.5612847222</x:v>
+      </x:c>
+      <x:c r="C90" s="2">
+        <x:v>45246.5639583333</x:v>
+      </x:c>
+      <x:c r="D90" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E90" s="10" t="s"/>
+      <x:c r="F90" s="2"/>
+      <x:c r="G90" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H90" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I90" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J90" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K90" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L90" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M90" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N90" s="10" t="s">
+        <x:v>393</x:v>
+      </x:c>
+      <x:c r="O90" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P90" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q90" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R90" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S90" s="10" t="s">
+        <x:v>394</x:v>
+      </x:c>
+      <x:c r="T90" s="10" t="s">
+        <x:v>395</x:v>
+      </x:c>
+      <x:c r="U90">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V90" s="10" t="s">
+        <x:v>396</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" hidden="0">
+      <x:c r="A91">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="B91" s="2">
+        <x:v>45246.5663657407</x:v>
+      </x:c>
+      <x:c r="C91" s="2">
+        <x:v>45246.5684953704</x:v>
+      </x:c>
+      <x:c r="D91" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E91" s="10" t="s"/>
+      <x:c r="F91" s="2"/>
+      <x:c r="G91" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H91" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I91" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J91" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K91" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L91" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M91" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N91" s="10" t="s">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="O91" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P91" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q91" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R91" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S91" s="10" t="s">
+        <x:v>398</x:v>
+      </x:c>
+      <x:c r="T91" s="10" t="s">
+        <x:v>399</x:v>
+      </x:c>
+      <x:c r="U91">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="V91" s="10" t="s">
+        <x:v>400</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" hidden="0">
+      <x:c r="A92">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B92" s="2">
+        <x:v>45246.5732986111</x:v>
+      </x:c>
+      <x:c r="C92" s="2">
+        <x:v>45246.5757175926</x:v>
+      </x:c>
+      <x:c r="D92" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E92" s="10" t="s"/>
+      <x:c r="F92" s="2"/>
+      <x:c r="G92" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H92" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I92" s="7" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J92" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K92" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L92" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M92" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N92" s="10" t="s">
+        <x:v>401</x:v>
+      </x:c>
+      <x:c r="O92" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P92" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q92" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="R92" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S92" s="10" t="s">
+        <x:v>402</x:v>
+      </x:c>
+      <x:c r="T92" s="10" t="s">
+        <x:v>403</x:v>
+      </x:c>
+      <x:c r="U92">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="V92" s="10" t="s"/>
+    </x:row>
+    <x:row r="93" hidden="0">
+      <x:c r="A93">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="B93" s="2">
+        <x:v>45246.5747916667</x:v>
+      </x:c>
+      <x:c r="C93" s="2">
+        <x:v>45246.5765046296</x:v>
+      </x:c>
+      <x:c r="D93" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E93" s="10" t="s"/>
+      <x:c r="F93" s="2"/>
+      <x:c r="G93" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H93" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I93" s="7" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="J93" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K93" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L93" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M93" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="N93" s="10" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="O93" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P93" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="Q93" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R93" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S93" s="10" t="s">
+        <x:v>404</x:v>
+      </x:c>
+      <x:c r="T93" s="10" t="s">
+        <x:v>405</x:v>
+      </x:c>
+      <x:c r="U93">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V93" s="10" t="s">
+        <x:v>406</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" hidden="0">
+      <x:c r="A94">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="B94" s="2">
+        <x:v>45246.5780902778</x:v>
+      </x:c>
+      <x:c r="C94" s="2">
+        <x:v>45246.5802083333</x:v>
+      </x:c>
+      <x:c r="D94" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E94" s="10" t="s"/>
+      <x:c r="F94" s="2"/>
+      <x:c r="G94" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H94" s="10" t="s">
+        <x:v>407</x:v>
+      </x:c>
+      <x:c r="I94" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J94" s="10" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="K94" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L94" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M94" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N94" s="10" t="s">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="O94" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P94" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q94" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R94" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S94" s="10" t="s">
+        <x:v>408</x:v>
+      </x:c>
+      <x:c r="T94" s="10" t="s"/>
+      <x:c r="U94">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V94" s="10" t="s">
+        <x:v>409</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" hidden="0">
+      <x:c r="A95">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B95" s="2">
+        <x:v>45246.5778240741</x:v>
+      </x:c>
+      <x:c r="C95" s="2">
+        <x:v>45246.5807407407</x:v>
+      </x:c>
+      <x:c r="D95" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E95" s="10" t="s"/>
+      <x:c r="F95" s="2"/>
+      <x:c r="G95" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H95" s="10" t="s">
+        <x:v>410</x:v>
+      </x:c>
+      <x:c r="I95" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J95" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K95" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L95" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M95" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N95" s="10" t="s">
+        <x:v>411</x:v>
+      </x:c>
+      <x:c r="O95" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P95" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q95" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R95" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S95" s="10" t="s">
+        <x:v>412</x:v>
+      </x:c>
+      <x:c r="T95" s="10" t="s">
+        <x:v>413</x:v>
+      </x:c>
+      <x:c r="U95">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="V95" s="10" t="s">
+        <x:v>414</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" hidden="0">
+      <x:c r="A96">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="B96" s="2">
+        <x:v>45246.5450925926</x:v>
+      </x:c>
+      <x:c r="C96" s="2">
+        <x:v>45246.586400463</x:v>
+      </x:c>
+      <x:c r="D96" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E96" s="10" t="s"/>
+      <x:c r="F96" s="2"/>
+      <x:c r="G96" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H96" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I96" s="7" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="J96" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K96" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L96" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M96" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N96" s="10" t="s">
+        <x:v>415</x:v>
+      </x:c>
+      <x:c r="O96" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P96" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q96" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R96" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S96" s="10" t="s">
+        <x:v>416</x:v>
+      </x:c>
+      <x:c r="T96" s="10" t="s">
+        <x:v>417</x:v>
+      </x:c>
+      <x:c r="U96">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V96" s="10" t="s">
+        <x:v>418</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" hidden="0">
+      <x:c r="A97">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B97" s="2">
+        <x:v>45246.5846527778</x:v>
+      </x:c>
+      <x:c r="C97" s="2">
+        <x:v>45246.5868865741</x:v>
+      </x:c>
+      <x:c r="D97" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E97" s="10" t="s"/>
+      <x:c r="F97" s="2"/>
+      <x:c r="G97" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H97" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="I97" s="7" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J97" s="10" t="s">
+        <x:v>419</x:v>
+      </x:c>
+      <x:c r="K97" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L97" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M97" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N97" s="10" t="s">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="O97" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P97" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q97" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R97" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="S97" s="10" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="T97" s="10" t="s">
+        <x:v>421</x:v>
+      </x:c>
+      <x:c r="U97">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V97" s="10" t="s">
+        <x:v>422</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" hidden="0">
+      <x:c r="A98">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="B98" s="2">
+        <x:v>45246.5847337963</x:v>
+      </x:c>
+      <x:c r="C98" s="2">
+        <x:v>45246.5882060185</x:v>
+      </x:c>
+      <x:c r="D98" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E98" s="10" t="s"/>
+      <x:c r="F98" s="2"/>
+      <x:c r="G98" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H98" s="10" t="s">
+        <x:v>423</x:v>
+      </x:c>
+      <x:c r="I98" s="7" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="J98" s="10" t="s">
+        <x:v>424</x:v>
+      </x:c>
+      <x:c r="K98" s="10" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="L98" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M98" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N98" s="10" t="s">
+        <x:v>425</x:v>
+      </x:c>
+      <x:c r="O98" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P98" s="10" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="Q98" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R98" s="10" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="S98" s="10" t="s">
+        <x:v>426</x:v>
+      </x:c>
+      <x:c r="T98" s="10" t="s">
+        <x:v>427</x:v>
+      </x:c>
+      <x:c r="U98">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="V98" s="10" t="s">
+        <x:v>428</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" hidden="0">
+      <x:c r="A99">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B99" s="2">
+        <x:v>45246.5845138889</x:v>
+      </x:c>
+      <x:c r="C99" s="2">
+        <x:v>45246.5883333333</x:v>
+      </x:c>
+      <x:c r="D99" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E99" s="10" t="s"/>
+      <x:c r="F99" s="2"/>
+      <x:c r="G99" s="10" t="s">
+        <x:v>347</x:v>
+      </x:c>
+      <x:c r="H99" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I99" s="7" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="J99" s="10" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="K99" s="10" t="s">
+        <x:v>355</x:v>
+      </x:c>
+      <x:c r="L99" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M99" s="10" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N99" s="10" t="s">
+        <x:v>429</x:v>
+      </x:c>
+      <x:c r="O99" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P99" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q99" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R99" s="10" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="S99" s="10" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="T99" s="10" t="s">
+        <x:v>430</x:v>
+      </x:c>
+      <x:c r="U99">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V99" s="10" t="s">
+        <x:v>431</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" hidden="0">
+      <x:c r="A100">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="B100" s="2">
+        <x:v>45246.5883564815</x:v>
+      </x:c>
+      <x:c r="C100" s="2">
+        <x:v>45246.5916203704</x:v>
+      </x:c>
+      <x:c r="D100" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E100" s="10" t="s"/>
+      <x:c r="F100" s="2"/>
+      <x:c r="G100" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H100" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I100" s="7" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="J100" s="10" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="K100" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L100" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M100" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N100" s="10" t="s">
+        <x:v>432</x:v>
+      </x:c>
+      <x:c r="O100" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P100" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q100" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R100" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S100" s="10" t="s">
+        <x:v>433</x:v>
+      </x:c>
+      <x:c r="T100" s="10" t="s">
+        <x:v>434</x:v>
+      </x:c>
+      <x:c r="U100">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="V100" s="10" t="s">
+        <x:v>435</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" hidden="0">
+      <x:c r="A101">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="B101" s="2">
+        <x:v>45246.5881018518</x:v>
+      </x:c>
+      <x:c r="C101" s="2">
+        <x:v>45246.5922800926</x:v>
+      </x:c>
+      <x:c r="D101" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E101" s="10" t="s"/>
+      <x:c r="F101" s="2"/>
+      <x:c r="G101" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H101" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I101" s="7" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="J101" s="10" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="K101" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L101" s="10" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="M101" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N101" s="10" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="O101" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P101" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q101" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R101" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S101" s="10" t="s">
+        <x:v>437</x:v>
+      </x:c>
+      <x:c r="T101" s="10" t="s">
+        <x:v>438</x:v>
+      </x:c>
+      <x:c r="U101">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V101" s="10" t="s">
+        <x:v>439</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" hidden="0">
+      <x:c r="A102">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="B102" s="2">
+        <x:v>45246.5921296296</x:v>
+      </x:c>
+      <x:c r="C102" s="2">
+        <x:v>45246.5930324074</x:v>
+      </x:c>
+      <x:c r="D102" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E102" s="10" t="s"/>
+      <x:c r="F102" s="2"/>
+      <x:c r="G102" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H102" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I102" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J102" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K102" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L102" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M102" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N102" s="10" t="s"/>
+      <x:c r="O102" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="P102" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q102" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R102" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S102" s="10" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="T102" s="10" t="s">
+        <x:v>441</x:v>
+      </x:c>
+      <x:c r="U102">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="V102" s="10" t="s">
+        <x:v>442</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" hidden="0">
+      <x:c r="A103">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="B103" s="2">
+        <x:v>45246.5889236111</x:v>
+      </x:c>
+      <x:c r="C103" s="2">
+        <x:v>45246.5951157407</x:v>
+      </x:c>
+      <x:c r="D103" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E103" s="10" t="s"/>
+      <x:c r="F103" s="2"/>
+      <x:c r="G103" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H103" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I103" s="7" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="J103" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K103" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L103" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M103" s="10" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="N103" s="10" t="s"/>
+      <x:c r="O103" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P103" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q103" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R103" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="S103" s="10" t="s">
+        <x:v>443</x:v>
+      </x:c>
+      <x:c r="T103" s="10" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="U103">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V103" s="10" t="s">
+        <x:v>445</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" hidden="0">
+      <x:c r="A104">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B104" s="2">
+        <x:v>45246.5978356481</x:v>
+      </x:c>
+      <x:c r="C104" s="2">
+        <x:v>45246.5988541667</x:v>
+      </x:c>
+      <x:c r="D104" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E104" s="10" t="s"/>
+      <x:c r="F104" s="2"/>
+      <x:c r="G104" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H104" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I104" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J104" s="10" t="s">
+        <x:v>354</x:v>
+      </x:c>
+      <x:c r="K104" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L104" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M104" s="10" t="s">
+        <x:v>446</x:v>
+      </x:c>
+      <x:c r="N104" s="10" t="s">
+        <x:v>447</x:v>
+      </x:c>
+      <x:c r="O104" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P104" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q104" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="R104" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S104" s="10" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="T104" s="10" t="s">
+        <x:v>449</x:v>
+      </x:c>
+      <x:c r="U104">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V104" s="10" t="s">
+        <x:v>450</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" hidden="0">
+      <x:c r="A105">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="B105" s="2">
+        <x:v>45246.5946643518</x:v>
+      </x:c>
+      <x:c r="C105" s="2">
+        <x:v>45246.5988773148</x:v>
+      </x:c>
+      <x:c r="D105" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E105" s="10" t="s"/>
+      <x:c r="F105" s="2"/>
+      <x:c r="G105" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H105" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I105" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J105" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K105" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L105" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M105" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N105" s="10" t="s">
+        <x:v>451</x:v>
+      </x:c>
+      <x:c r="O105" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P105" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q105" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R105" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S105" s="10" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="T105" s="10" t="s"/>
+      <x:c r="U105">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="V105" s="10" t="s"/>
+    </x:row>
+    <x:row r="106" hidden="0">
+      <x:c r="A106">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="B106" s="2">
+        <x:v>45246.5944212963</x:v>
+      </x:c>
+      <x:c r="C106" s="2">
+        <x:v>45246.5996990741</x:v>
+      </x:c>
+      <x:c r="D106" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E106" s="10" t="s"/>
+      <x:c r="F106" s="2"/>
+      <x:c r="G106" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H106" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I106" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J106" s="10" t="s">
+        <x:v>453</x:v>
+      </x:c>
+      <x:c r="K106" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L106" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M106" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N106" s="10" t="s">
+        <x:v>454</x:v>
+      </x:c>
+      <x:c r="O106" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P106" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q106" s="10" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="R106" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S106" s="10" t="s">
+        <x:v>455</x:v>
+      </x:c>
+      <x:c r="T106" s="10" t="s">
+        <x:v>456</x:v>
+      </x:c>
+      <x:c r="U106">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V106" s="10" t="s">
+        <x:v>457</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" hidden="0">
+      <x:c r="A107">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="B107" s="2">
+        <x:v>45246.6018518518</x:v>
+      </x:c>
+      <x:c r="C107" s="2">
+        <x:v>45246.6032638889</x:v>
+      </x:c>
+      <x:c r="D107" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E107" s="10" t="s"/>
+      <x:c r="F107" s="2"/>
+      <x:c r="G107" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H107" s="10" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I107" s="7" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="J107" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K107" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L107" s="10" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="M107" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N107" s="10" t="s">
+        <x:v>458</x:v>
+      </x:c>
+      <x:c r="O107" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P107" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q107" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R107" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S107" s="10" t="s">
+        <x:v>459</x:v>
+      </x:c>
+      <x:c r="T107" s="10" t="s">
+        <x:v>460</x:v>
+      </x:c>
+      <x:c r="U107">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="V107" s="10" t="s">
+        <x:v>461</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" hidden="0">
+      <x:c r="A108">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="B108" s="2">
+        <x:v>45246.6017824074</x:v>
+      </x:c>
+      <x:c r="C108" s="2">
+        <x:v>45246.6038078704</x:v>
+      </x:c>
+      <x:c r="D108" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E108" s="10" t="s"/>
+      <x:c r="F108" s="2"/>
+      <x:c r="G108" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H108" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I108" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J108" s="10" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="K108" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L108" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M108" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N108" s="10" t="s">
+        <x:v>462</x:v>
+      </x:c>
+      <x:c r="O108" s="10" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P108" s="10" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="Q108" s="10" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="R108" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S108" s="10" t="s">
+        <x:v>463</x:v>
+      </x:c>
+      <x:c r="T108" s="10" t="s">
+        <x:v>464</x:v>
+      </x:c>
+      <x:c r="U108">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V108" s="10" t="s">
+        <x:v>465</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" hidden="0">
+      <x:c r="A109">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="B109" s="2">
+        <x:v>45246.6032523148</x:v>
+      </x:c>
+      <x:c r="C109" s="2">
+        <x:v>45246.6045949074</x:v>
+      </x:c>
+      <x:c r="D109" s="10" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E109" s="10" t="s"/>
+      <x:c r="F109" s="2"/>
+      <x:c r="G109" s="10" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H109" s="10" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="I109" s="7" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="J109" s="10" t="s">
+        <x:v>231</x:v>
+      </x:c>
+      <x:c r="K109" s="10" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L109" s="10" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="M109" s="10" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="N109" s="10" t="s">
+        <x:v>466</x:v>
+      </x:c>
+      <x:c r="O109" s="10" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="P109" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="Q109" s="10" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="R109" s="10" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="S109" s="10" t="s">
+        <x:v>467</x:v>
+      </x:c>
+      <x:c r="T109" s="10" t="s">
+        <x:v>468</x:v>
+      </x:c>
+      <x:c r="U109">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="V109" s="10" t="s">
+        <x:v>469</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R156eec764ef64612"/>
+    <x:tablePart r:id="R65661c6f6c754c89"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>